<commit_message>
Adding/moving preprocessed files to "preprocessed" folder.
</commit_message>
<xml_diff>
--- a/preprocessed/regions200.xlsx
+++ b/preprocessed/regions200.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t xml:space="preserve">chr</t>
   </si>
@@ -32,6 +32,12 @@
     <t xml:space="preserve">SNP</t>
   </si>
   <si>
+    <t xml:space="preserve">refseq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crispick</t>
+  </si>
+  <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
@@ -41,271 +47,544 @@
     <t xml:space="preserve">rs71475909</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000011.9:+:47377184-47377382</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs10838702</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:47410789-47410987</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1377416</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:47416647-47416845</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs11039225</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:47430500-47430698</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs10897011|rs11230180</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:59961328-59961585</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs7936120</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:60000475-60000673</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs718376</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:60002836-60003034</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs672399</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:60020013-60020211</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs7128450</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:60031171-60031369</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs7930318|rs4938932</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:60033272-60033547</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1237999</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:85814931-85815129</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs474479|rs598726</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:85828449-85828650</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs10792832</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:85867776-85867974</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs74685827</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000011.9:+:121352978-121353176</t>
+  </si>
+  <si>
     <t xml:space="preserve">8</t>
   </si>
   <si>
     <t xml:space="preserve">rs28834970</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000008.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000008.10:+:27195022-27195220</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs73223431</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000008.10:+:27219888-27220086</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs2279590</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000008.10:+:27456154-27456352</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1532276|rs1532277|rs1532278</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000008.10:+:27466058-27466414</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs34173062</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000008.10:+:145158508-145158706</t>
+  </si>
+  <si>
     <t xml:space="preserve">16</t>
   </si>
   <si>
     <t xml:space="preserve">rs4318227</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000016.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000016.9:+:29984740-29984938</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1140239</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000016.9:+:30021303-30021501</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1549299</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000016.9:+:31154047-31154245</t>
+  </si>
+  <si>
     <t xml:space="preserve">6</t>
   </si>
   <si>
     <t xml:space="preserve">rs9271579|rs9271580</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000006.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000006.11:+:32590538-32590740</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs9271608</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000006.11:+:32591489-32591687</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs785135</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000006.11:+:114637332-114637530</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs785143</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000006.11:+:114645138-114645336</t>
+  </si>
+  <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
     <t xml:space="preserve">rs4989024</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000017.10:+:1639620-1639818</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1317708|rs874424</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:1639866-1640133</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs8077638|rs34962442|rs62090051</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:1640430-1640892</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs2287322</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:1640936-1641134</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1310</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:1641616-1641814</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs2070863</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:1648403-1648601</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs2075659</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:18044493-18044691</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs2072653</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:18044999-18045197</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs58804619</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:18090555-18090753</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs199528</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:44843037-44843235</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs199523|rs199524</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:44848339-44848616</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs70602</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:44859616-44859814</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs916888</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000017.10:+:44863034-44863232</t>
+  </si>
+  <si>
     <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">rs113598561</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000019.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000019.9:+:1819135-1819333</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs2287921</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000019.9:+:49228173-49228371</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1761452</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000019.9:+:54815267-54815465</t>
+  </si>
+  <si>
     <t xml:space="preserve">7</t>
   </si>
   <si>
     <t xml:space="preserve">rs74504435</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000007.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000007.13:+:54949157-54949355</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs12539172</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000007.13:+:100091696-100091894</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs3935067</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000007.13:+:143104232-143104430</t>
+  </si>
+  <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">rs58250526</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000012.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000012.11:+:113591338-113591536</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs73208737</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000012.11:+:113634956-113635154</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs7297749|rs76097225</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000012.11:+:113659522-113659851</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs78810900</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000012.11:+:113679499-113679697</t>
+  </si>
+  <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
     <t xml:space="preserve">rs9633740</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000010.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000010.10:+:82265172-82265370</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1870138|rs7080009</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000010.10:+:82269362-82269710</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs1870137</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000010.10:+:82269749-82269947</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs117148433</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000010.10:+:98017767-98017965</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs117699776</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000010.10:+:98048166-98048364</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs56029211</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000010.10:+:124127891-124128089</t>
+  </si>
+  <si>
     <t xml:space="preserve">9</t>
   </si>
   <si>
     <t xml:space="preserve">rs2777795</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000009.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000009.11:+:107672266-107672464</t>
+  </si>
+  <si>
     <t xml:space="preserve">20</t>
   </si>
   <si>
     <t xml:space="preserve">rs6064392</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000020.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000020.10:+:54984669-54984867</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs6024870</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000020.10:+:54997469-54997667</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs718022</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000020.10:+:55003366-55003564</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs76842328</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000020.10:+:55012893-55013091</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs927174</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000020.10:+:55015067-55015265</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs544475179|rs7274581</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000020.10:+:55018057-55018359</t>
+  </si>
+  <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">rs17125798|rs1952088</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000014.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000014.8:+:53319733-53320004</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs11629431</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000014.8:+:53320429-53320627</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs7149638</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000014.8:+:53346832-53347030</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs8003334|rs8019279|rs8019585</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000014.8:+:53374678-53375066</t>
+  </si>
+  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">rs6733839|rs34779859</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000002.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000002.11:+:127892669-127892909</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs72934512</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000002.11:+:203926172-203926370</t>
+  </si>
+  <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">rs2452758</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000005.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000005.9:+:86181604-86181802</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs56363426</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000005.9:+:86300359-86300557</t>
+  </si>
+  <si>
     <t xml:space="preserve">rs3087616</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000005.9:+:156513183-156513381</t>
+  </si>
+  <si>
     <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">rs332261|rs332262</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000015.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000015.9:+:64382798-64383128</t>
+  </si>
+  <si>
     <t xml:space="preserve">21</t>
   </si>
   <si>
     <t xml:space="preserve">rs469420</t>
   </si>
   <si>
+    <t xml:space="preserve">NC_000021.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000021.8:+:27541845-27542043</t>
+  </si>
+  <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">rs2245466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000004.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_000004.11:+:40198747-40198945</t>
   </si>
 </sst>
 </file>
@@ -656,10 +935,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>47377184</v>
@@ -671,15 +956,21 @@
         <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>47410789</v>
@@ -691,15 +982,21 @@
         <v>199</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
         <v>47416647</v>
@@ -711,15 +1008,21 @@
         <v>199</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="n">
         <v>47430500</v>
@@ -731,15 +1034,21 @@
         <v>199</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
         <v>59961328</v>
@@ -751,15 +1060,21 @@
         <v>258</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="n">
         <v>60000475</v>
@@ -771,15 +1086,21 @@
         <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
         <v>60002836</v>
@@ -791,15 +1112,21 @@
         <v>199</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
         <v>60020013</v>
@@ -811,15 +1138,21 @@
         <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>60031171</v>
@@ -831,15 +1164,21 @@
         <v>199</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="n">
         <v>60033272</v>
@@ -851,15 +1190,21 @@
         <v>276</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="n">
         <v>85814931</v>
@@ -871,15 +1216,21 @@
         <v>199</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="n">
         <v>85828449</v>
@@ -891,15 +1242,21 @@
         <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" t="n">
         <v>85867776</v>
@@ -911,15 +1268,21 @@
         <v>199</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15" t="n">
         <v>121352978</v>
@@ -931,15 +1294,21 @@
         <v>199</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B16" t="n">
         <v>27195022</v>
@@ -951,15 +1320,21 @@
         <v>199</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B17" t="n">
         <v>27219888</v>
@@ -971,15 +1346,21 @@
         <v>199</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B18" t="n">
         <v>27456154</v>
@@ -991,15 +1372,21 @@
         <v>199</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B19" t="n">
         <v>27466058</v>
@@ -1011,15 +1398,21 @@
         <v>357</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B20" t="n">
         <v>145158508</v>
@@ -1031,15 +1424,21 @@
         <v>199</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B21" t="n">
         <v>29984740</v>
@@ -1051,15 +1450,21 @@
         <v>199</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B22" t="n">
         <v>30021303</v>
@@ -1071,15 +1476,21 @@
         <v>199</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B23" t="n">
         <v>31154047</v>
@@ -1091,15 +1502,21 @@
         <v>199</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B24" t="n">
         <v>32590538</v>
@@ -1111,15 +1528,21 @@
         <v>203</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B25" t="n">
         <v>32591489</v>
@@ -1131,15 +1554,21 @@
         <v>199</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>63</v>
+      </c>
+      <c r="G25" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B26" t="n">
         <v>114637332</v>
@@ -1151,15 +1580,21 @@
         <v>199</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+      <c r="G26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B27" t="n">
         <v>114645138</v>
@@ -1171,15 +1606,21 @@
         <v>199</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B28" t="n">
         <v>1639620</v>
@@ -1191,15 +1632,21 @@
         <v>199</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>70</v>
+      </c>
+      <c r="G28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B29" t="n">
         <v>1639866</v>
@@ -1211,15 +1658,21 @@
         <v>268</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B30" t="n">
         <v>1640430</v>
@@ -1231,15 +1684,21 @@
         <v>463</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>40</v>
+        <v>75</v>
+      </c>
+      <c r="G30" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B31" t="n">
         <v>1640936</v>
@@ -1251,15 +1710,21 @@
         <v>199</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>41</v>
+        <v>77</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B32" t="n">
         <v>1641616</v>
@@ -1271,15 +1736,21 @@
         <v>199</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>79</v>
+      </c>
+      <c r="G32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H32" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B33" t="n">
         <v>1648403</v>
@@ -1291,15 +1762,21 @@
         <v>199</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>43</v>
+        <v>81</v>
+      </c>
+      <c r="G33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H33" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B34" t="n">
         <v>18044493</v>
@@ -1311,15 +1788,21 @@
         <v>199</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>83</v>
+      </c>
+      <c r="G34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B35" t="n">
         <v>18044999</v>
@@ -1331,15 +1814,21 @@
         <v>199</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>45</v>
+        <v>85</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B36" t="n">
         <v>18090555</v>
@@ -1351,15 +1840,21 @@
         <v>199</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>87</v>
+      </c>
+      <c r="G36" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B37" t="n">
         <v>44843037</v>
@@ -1371,15 +1866,21 @@
         <v>199</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>47</v>
+        <v>89</v>
+      </c>
+      <c r="G37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B38" t="n">
         <v>44848339</v>
@@ -1391,15 +1892,21 @@
         <v>278</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>48</v>
+        <v>91</v>
+      </c>
+      <c r="G38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H38" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B39" t="n">
         <v>44859616</v>
@@ -1411,15 +1918,21 @@
         <v>199</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>49</v>
+        <v>93</v>
+      </c>
+      <c r="G39" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B40" t="n">
         <v>44863034</v>
@@ -1431,15 +1944,21 @@
         <v>199</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>50</v>
+        <v>95</v>
+      </c>
+      <c r="G40" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B41" t="n">
         <v>1819135</v>
@@ -1451,15 +1970,21 @@
         <v>199</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>52</v>
+        <v>98</v>
+      </c>
+      <c r="G41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B42" t="n">
         <v>49228173</v>
@@ -1471,15 +1996,21 @@
         <v>199</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>53</v>
+        <v>101</v>
+      </c>
+      <c r="G42" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B43" t="n">
         <v>54815267</v>
@@ -1491,15 +2022,21 @@
         <v>199</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>54</v>
+        <v>103</v>
+      </c>
+      <c r="G43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H43" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B44" t="n">
         <v>54949157</v>
@@ -1511,15 +2048,21 @@
         <v>199</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>106</v>
+      </c>
+      <c r="G44" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B45" t="n">
         <v>100091696</v>
@@ -1531,15 +2074,21 @@
         <v>199</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>57</v>
+        <v>109</v>
+      </c>
+      <c r="G45" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B46" t="n">
         <v>143104232</v>
@@ -1551,15 +2100,21 @@
         <v>199</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F46" t="s">
-        <v>58</v>
+        <v>111</v>
+      </c>
+      <c r="G46" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B47" t="n">
         <v>113591338</v>
@@ -1571,15 +2126,21 @@
         <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F47" t="s">
-        <v>60</v>
+        <v>114</v>
+      </c>
+      <c r="G47" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B48" t="n">
         <v>113634956</v>
@@ -1591,15 +2152,21 @@
         <v>199</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F48" t="s">
-        <v>61</v>
+        <v>117</v>
+      </c>
+      <c r="G48" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B49" t="n">
         <v>113659522</v>
@@ -1611,15 +2178,21 @@
         <v>330</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F49" t="s">
-        <v>62</v>
+        <v>119</v>
+      </c>
+      <c r="G49" t="s">
+        <v>115</v>
+      </c>
+      <c r="H49" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B50" t="n">
         <v>113679499</v>
@@ -1631,15 +2204,21 @@
         <v>199</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>63</v>
+        <v>121</v>
+      </c>
+      <c r="G50" t="s">
+        <v>115</v>
+      </c>
+      <c r="H50" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B51" t="n">
         <v>82265172</v>
@@ -1651,15 +2230,21 @@
         <v>199</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F51" t="s">
-        <v>65</v>
+        <v>124</v>
+      </c>
+      <c r="G51" t="s">
+        <v>125</v>
+      </c>
+      <c r="H51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B52" t="n">
         <v>82269362</v>
@@ -1671,15 +2256,21 @@
         <v>349</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>66</v>
+        <v>127</v>
+      </c>
+      <c r="G52" t="s">
+        <v>125</v>
+      </c>
+      <c r="H52" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B53" t="n">
         <v>82269749</v>
@@ -1691,15 +2282,21 @@
         <v>199</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F53" t="s">
-        <v>67</v>
+        <v>129</v>
+      </c>
+      <c r="G53" t="s">
+        <v>125</v>
+      </c>
+      <c r="H53" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B54" t="n">
         <v>98017767</v>
@@ -1711,15 +2308,21 @@
         <v>199</v>
       </c>
       <c r="E54" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F54" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="G54" t="s">
+        <v>125</v>
+      </c>
+      <c r="H54" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B55" t="n">
         <v>98048166</v>
@@ -1731,15 +2334,21 @@
         <v>199</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F55" t="s">
-        <v>69</v>
+        <v>133</v>
+      </c>
+      <c r="G55" t="s">
+        <v>125</v>
+      </c>
+      <c r="H55" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B56" t="n">
         <v>124127891</v>
@@ -1751,15 +2360,21 @@
         <v>199</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F56" t="s">
-        <v>70</v>
+        <v>135</v>
+      </c>
+      <c r="G56" t="s">
+        <v>125</v>
+      </c>
+      <c r="H56" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="B57" t="n">
         <v>107672266</v>
@@ -1771,15 +2386,21 @@
         <v>199</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F57" t="s">
-        <v>72</v>
+        <v>138</v>
+      </c>
+      <c r="G57" t="s">
+        <v>139</v>
+      </c>
+      <c r="H57" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B58" t="n">
         <v>54984669</v>
@@ -1791,15 +2412,21 @@
         <v>199</v>
       </c>
       <c r="E58" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F58" t="s">
-        <v>74</v>
+        <v>142</v>
+      </c>
+      <c r="G58" t="s">
+        <v>143</v>
+      </c>
+      <c r="H58" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B59" t="n">
         <v>54997469</v>
@@ -1811,15 +2438,21 @@
         <v>199</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F59" t="s">
-        <v>75</v>
+        <v>145</v>
+      </c>
+      <c r="G59" t="s">
+        <v>143</v>
+      </c>
+      <c r="H59" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B60" t="n">
         <v>55003366</v>
@@ -1831,15 +2464,21 @@
         <v>199</v>
       </c>
       <c r="E60" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F60" t="s">
-        <v>76</v>
+        <v>147</v>
+      </c>
+      <c r="G60" t="s">
+        <v>143</v>
+      </c>
+      <c r="H60" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B61" t="n">
         <v>55012893</v>
@@ -1851,15 +2490,21 @@
         <v>199</v>
       </c>
       <c r="E61" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>77</v>
+        <v>149</v>
+      </c>
+      <c r="G61" t="s">
+        <v>143</v>
+      </c>
+      <c r="H61" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B62" t="n">
         <v>55015067</v>
@@ -1871,15 +2516,21 @@
         <v>199</v>
       </c>
       <c r="E62" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F62" t="s">
-        <v>78</v>
+        <v>151</v>
+      </c>
+      <c r="G62" t="s">
+        <v>143</v>
+      </c>
+      <c r="H62" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B63" t="n">
         <v>55018057</v>
@@ -1891,15 +2542,21 @@
         <v>303</v>
       </c>
       <c r="E63" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F63" t="s">
-        <v>79</v>
+        <v>153</v>
+      </c>
+      <c r="G63" t="s">
+        <v>143</v>
+      </c>
+      <c r="H63" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="B64" t="n">
         <v>53319733</v>
@@ -1911,15 +2568,21 @@
         <v>272</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>81</v>
+        <v>156</v>
+      </c>
+      <c r="G64" t="s">
+        <v>157</v>
+      </c>
+      <c r="H64" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="B65" t="n">
         <v>53320429</v>
@@ -1931,15 +2594,21 @@
         <v>199</v>
       </c>
       <c r="E65" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>82</v>
+        <v>159</v>
+      </c>
+      <c r="G65" t="s">
+        <v>157</v>
+      </c>
+      <c r="H65" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="B66" t="n">
         <v>53346832</v>
@@ -1951,15 +2620,21 @@
         <v>199</v>
       </c>
       <c r="E66" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>83</v>
+        <v>161</v>
+      </c>
+      <c r="G66" t="s">
+        <v>157</v>
+      </c>
+      <c r="H66" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="B67" t="n">
         <v>53374678</v>
@@ -1971,15 +2646,21 @@
         <v>389</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F67" t="s">
-        <v>84</v>
+        <v>163</v>
+      </c>
+      <c r="G67" t="s">
+        <v>157</v>
+      </c>
+      <c r="H67" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="B68" t="n">
         <v>127892669</v>
@@ -1991,15 +2672,21 @@
         <v>241</v>
       </c>
       <c r="E68" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F68" t="s">
-        <v>86</v>
+        <v>166</v>
+      </c>
+      <c r="G68" t="s">
+        <v>167</v>
+      </c>
+      <c r="H68" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="B69" t="n">
         <v>203926172</v>
@@ -2011,15 +2698,21 @@
         <v>199</v>
       </c>
       <c r="E69" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F69" t="s">
-        <v>87</v>
+        <v>169</v>
+      </c>
+      <c r="G69" t="s">
+        <v>167</v>
+      </c>
+      <c r="H69" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="B70" t="n">
         <v>86181604</v>
@@ -2031,15 +2724,21 @@
         <v>199</v>
       </c>
       <c r="E70" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F70" t="s">
-        <v>89</v>
+        <v>172</v>
+      </c>
+      <c r="G70" t="s">
+        <v>173</v>
+      </c>
+      <c r="H70" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="B71" t="n">
         <v>86300359</v>
@@ -2051,15 +2750,21 @@
         <v>199</v>
       </c>
       <c r="E71" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F71" t="s">
-        <v>90</v>
+        <v>175</v>
+      </c>
+      <c r="G71" t="s">
+        <v>173</v>
+      </c>
+      <c r="H71" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="B72" t="n">
         <v>156513183</v>
@@ -2071,15 +2776,21 @@
         <v>199</v>
       </c>
       <c r="E72" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F72" t="s">
-        <v>91</v>
+        <v>177</v>
+      </c>
+      <c r="G72" t="s">
+        <v>173</v>
+      </c>
+      <c r="H72" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>179</v>
       </c>
       <c r="B73" t="n">
         <v>64382798</v>
@@ -2091,15 +2802,21 @@
         <v>331</v>
       </c>
       <c r="E73" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F73" t="s">
-        <v>93</v>
+        <v>180</v>
+      </c>
+      <c r="G73" t="s">
+        <v>181</v>
+      </c>
+      <c r="H73" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="B74" t="n">
         <v>27541845</v>
@@ -2111,15 +2828,21 @@
         <v>199</v>
       </c>
       <c r="E74" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F74" t="s">
-        <v>95</v>
+        <v>184</v>
+      </c>
+      <c r="G74" t="s">
+        <v>185</v>
+      </c>
+      <c r="H74" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="B75" t="n">
         <v>40198747</v>
@@ -2131,10 +2854,16 @@
         <v>199</v>
       </c>
       <c r="E75" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F75" t="s">
-        <v>97</v>
+        <v>188</v>
+      </c>
+      <c r="G75" t="s">
+        <v>189</v>
+      </c>
+      <c r="H75" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>